<commit_message>
two more history variables removed + some progress in left commute proofs
</commit_message>
<xml_diff>
--- a/assignment/Paper/event-deps.xlsx
+++ b/assignment/Paper/event-deps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shabn\OneDrive\Documents\Zurich\University\Resesarch\distributed-database-transactions\assignment\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A22015-D57A-45F3-8700-995470A9DA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18CFEB5-2499-4FE1-B247-6220940EC00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5520" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>RegR k1</t>
   </si>
@@ -235,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -258,24 +258,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,25 +285,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,217 +588,233 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" style="3" customWidth="1"/>
-    <col min="2" max="10" width="4.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.90625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="14.7265625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
+    <col min="2" max="10" width="4.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="14.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12">
-        <v>2</v>
-      </c>
-      <c r="I3" s="12">
-        <v>1</v>
-      </c>
-      <c r="J3" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12">
-        <v>1</v>
-      </c>
-      <c r="J4" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12">
-        <v>2</v>
-      </c>
-      <c r="I7" s="12">
-        <v>2</v>
-      </c>
-      <c r="J7" s="12" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9">
+        <v>2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12">
-        <v>2</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12">
-        <v>2</v>
-      </c>
-      <c r="G8" s="12">
-        <v>2</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>2</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:20" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O12" s="1" t="s">
         <v>31</v>
       </c>
@@ -834,19 +831,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L17" s="3" t="s">
         <v>6</v>
       </c>
@@ -875,10 +875,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L19" s="3" t="s">
         <v>7</v>
       </c>
@@ -910,10 +910,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L21" s="3"/>
       <c r="O21" s="4" t="s">
         <v>13</v>
@@ -937,16 +937,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L25" s="2" t="s">
         <v>13</v>
       </c>
@@ -969,37 +969,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L29" s="3"/>
       <c r="N29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L30" s="3"/>
       <c r="N30" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L31" s="3"/>
       <c r="N31" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="12:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L32" s="3"/>
     </row>
-    <row r="36" spans="13:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M36" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>